<commit_message>
mejoras en el sistema de refacturación, se añade cambio de fecha, tipo de comproante y xlst, nuevo formato de excel
</commit_message>
<xml_diff>
--- a/storage/documents/Formato_Cargue_Facturas.xlsx
+++ b/storage/documents/Formato_Cargue_Facturas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\softlogy-micro\storage\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://softlogy-my.sharepoint.com/personal/jeremy_pedraza_softlogyco_com/Documents/Documents/Abril 21 2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672CD52B-C783-416E-84C0-CAF4F6288EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{672CD52B-C783-416E-84C0-CAF4F6288EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBAF4CB6-853B-4179-B5DC-7DE3D9C2632E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{141EF29D-D662-4900-BB9B-925A517980B9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{141EF29D-D662-4900-BB9B-925A517980B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Cargue" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5735" uniqueCount="1055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5737" uniqueCount="1057">
   <si>
     <t>Id</t>
   </si>
@@ -3201,10 +3201,16 @@
     <t>NumResolucion</t>
   </si>
   <si>
-    <t>AGREGAR MAS DATOS SI ES NECESARIO, NOTIFICAR A DESARRLLO PREVIAMENTE</t>
-  </si>
-  <si>
     <t>XML - EJEMPLO 👇👇 AGREGAR APARTIR DE LA FILA 2</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Tipo Comprobante</t>
+  </si>
+  <si>
+    <t>XSLT</t>
   </si>
 </sst>
 </file>
@@ -3220,12 +3226,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3240,10 +3252,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3578,10 +3591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F07C870-EE85-45CC-A34A-8D38994396B9}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,9 +3604,9 @@
     <col min="4" max="4" width="24.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -3604,11 +3617,17 @@
       <c r="D1" s="2" t="s">
         <v>1052</v>
       </c>
-      <c r="E1" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1051</v>
       </c>
@@ -3621,9 +3640,19 @@
       <c r="D2" s="2">
         <v>18764077890286</v>
       </c>
+      <c r="E2" s="1">
+        <v>45747</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>